<commit_message>
Combine linear models with simple SVM
</commit_message>
<xml_diff>
--- a/data_plan.xlsx
+++ b/data_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="104">
   <si>
     <t>Var Name</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>(NOTE: Coded as numeric; need to convert to factor)</t>
+  </si>
+  <si>
+    <t>consider making continuous</t>
+  </si>
+  <si>
+    <t>consider options</t>
+  </si>
+  <si>
+    <t>consider making continuous somehow or narrowing categories</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1156,7 +1165,7 @@
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1236,23 +1245,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -1260,7 +1275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1268,7 +1283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1276,7 +1291,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1284,7 +1299,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -1292,7 +1307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1300,7 +1315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1308,7 +1323,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1316,15 +1331,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1332,7 +1350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1340,7 +1358,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1348,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1356,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1364,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1372,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1380,7 +1398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1388,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1396,7 +1414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1404,7 +1422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>61</v>
       </c>

</xml_diff>